<commit_message>
Outline for rename of files.
git-svn-id: svn://136.177.114.72/svn_GW/webmod/trunk@9837 1feff8c3-07ed-0310-ac33-dd36852eb9cd
</commit_message>
<xml_diff>
--- a/pest/PestFiles.xlsx
+++ b/pest/PestFiles.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="133">
   <si>
     <t>AndChemLoads.ssf</t>
   </si>
@@ -279,12 +279,6 @@
     <t>Created by Pest</t>
   </si>
   <si>
-    <t>Based on pqi_andcrk.tpl</t>
-  </si>
-  <si>
-    <t>Based on params_andcrk.tpl</t>
-  </si>
-  <si>
     <t>Webmod output</t>
   </si>
   <si>
@@ -298,6 +292,138 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>New name</t>
+  </si>
+  <si>
+    <t>phreeq.lut</t>
+  </si>
+  <si>
+    <t>phreeqc_web.dat</t>
+  </si>
+  <si>
+    <t>webmod.exe</t>
+  </si>
+  <si>
+    <t>bas.chem.obs.ssf</t>
+  </si>
+  <si>
+    <t>bas.webmod.control</t>
+  </si>
+  <si>
+    <t>bas.hydro.dat</t>
+  </si>
+  <si>
+    <t>bas.chem.dat</t>
+  </si>
+  <si>
+    <t>bas.statvar</t>
+  </si>
+  <si>
+    <t>bas.hydro.obs.ssf</t>
+  </si>
+  <si>
+    <t>bas.params.tpl</t>
+  </si>
+  <si>
+    <t>bas.pqi.tpl</t>
+  </si>
+  <si>
+    <t>bas.par2par.dat.tpl</t>
+  </si>
+  <si>
+    <t>bas.par2par.dat</t>
+  </si>
+  <si>
+    <t>bas.pest_groups.txt</t>
+  </si>
+  <si>
+    <t>bas.pest_params.txt</t>
+  </si>
+  <si>
+    <t>bas.tsproc.dat.tpl</t>
+  </si>
+  <si>
+    <t>bas.tsproc.dat</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>bas.pst</t>
+  </si>
+  <si>
+    <t>bas.sim.out</t>
+  </si>
+  <si>
+    <t>bas.sim.out.ins</t>
+  </si>
+  <si>
+    <t>bas.jac</t>
+  </si>
+  <si>
+    <t>bas.jco</t>
+  </si>
+  <si>
+    <t>bas.jst</t>
+  </si>
+  <si>
+    <t>bas.mtt</t>
+  </si>
+  <si>
+    <t>bas.par</t>
+  </si>
+  <si>
+    <t>bas.prf</t>
+  </si>
+  <si>
+    <t>bas.rec</t>
+  </si>
+  <si>
+    <t>bas.rei</t>
+  </si>
+  <si>
+    <t>bas.res</t>
+  </si>
+  <si>
+    <t>bas.rmr</t>
+  </si>
+  <si>
+    <t>bas.rsd</t>
+  </si>
+  <si>
+    <t>bas.rst</t>
+  </si>
+  <si>
+    <t>bas.sen</t>
+  </si>
+  <si>
+    <t>bas.seo</t>
+  </si>
+  <si>
+    <t>bas.svd</t>
+  </si>
+  <si>
+    <t>bas.pqi</t>
+  </si>
+  <si>
+    <t>bas.params</t>
+  </si>
+  <si>
+    <t>Based on bas.params.tpl</t>
+  </si>
+  <si>
+    <t>Based on bas.pqi.tpl</t>
+  </si>
+  <si>
+    <t>bas.hydro.out</t>
+  </si>
+  <si>
+    <t>bas.chem.out</t>
+  </si>
+  <si>
+    <t>bas.topout</t>
   </si>
 </sst>
 </file>
@@ -616,24 +742,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="31.21875" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="36.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" customWidth="1"/>
+    <col min="3" max="4" width="31.21875" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
+    <col min="7" max="7" width="36.88671875" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -641,24 +767,27 @@
         <v>81</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -666,793 +795,986 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="E26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" t="s">
         <v>59</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>25</v>
+        <v>107</v>
       </c>
       <c r="E27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" t="s">
         <v>59</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="E28" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" t="s">
         <v>59</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" t="s">
+        <v>59</v>
+      </c>
+      <c r="G29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>101</v>
+      </c>
+      <c r="E30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" t="s">
+        <v>59</v>
+      </c>
+      <c r="G30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" t="s">
+        <v>59</v>
+      </c>
+      <c r="G31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" t="s">
+        <v>97</v>
+      </c>
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" t="s">
+        <v>72</v>
+      </c>
+      <c r="G33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" t="s">
+        <v>72</v>
+      </c>
+      <c r="F35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" t="s">
+        <v>110</v>
+      </c>
+      <c r="E36" t="s">
+        <v>72</v>
+      </c>
+      <c r="F36" t="s">
+        <v>58</v>
+      </c>
+      <c r="G36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" t="s">
+        <v>57</v>
+      </c>
+      <c r="E37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" t="s">
+        <v>109</v>
+      </c>
+      <c r="E38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" t="s">
+        <v>58</v>
+      </c>
+      <c r="G40" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" t="s">
+        <v>52</v>
+      </c>
+      <c r="E41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" t="s">
+        <v>58</v>
+      </c>
+      <c r="G41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" t="s">
+        <v>94</v>
+      </c>
+      <c r="E42" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" t="s">
+        <v>32</v>
+      </c>
+      <c r="G42" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" t="s">
+        <v>92</v>
+      </c>
+      <c r="E43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G43" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" t="s">
+        <v>111</v>
+      </c>
+      <c r="E45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" t="s">
+        <v>112</v>
+      </c>
+      <c r="E46" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47" t="s">
+        <v>113</v>
+      </c>
+      <c r="E47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" t="s">
+        <v>114</v>
+      </c>
+      <c r="E48" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>38</v>
+      </c>
+      <c r="D49" t="s">
+        <v>115</v>
+      </c>
+      <c r="E49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" t="s">
+        <v>116</v>
+      </c>
+      <c r="E50" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>41</v>
+      </c>
+      <c r="D51" t="s">
+        <v>117</v>
+      </c>
+      <c r="E51" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>42</v>
+      </c>
+      <c r="D52" t="s">
+        <v>118</v>
+      </c>
+      <c r="E52" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>43</v>
+      </c>
+      <c r="D53" t="s">
+        <v>119</v>
+      </c>
+      <c r="E53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>44</v>
+      </c>
+      <c r="D54" t="s">
+        <v>120</v>
+      </c>
+      <c r="E54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>45</v>
+      </c>
+      <c r="D55" t="s">
+        <v>121</v>
+      </c>
+      <c r="E55" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>46</v>
+      </c>
+      <c r="D56" t="s">
+        <v>122</v>
+      </c>
+      <c r="E56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>47</v>
+      </c>
+      <c r="D57" t="s">
+        <v>123</v>
+      </c>
+      <c r="E57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
+        <v>48</v>
+      </c>
+      <c r="D58" t="s">
+        <v>124</v>
+      </c>
+      <c r="E58" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>50</v>
+      </c>
+      <c r="D59" t="s">
+        <v>125</v>
+      </c>
+      <c r="E59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>27</v>
+      </c>
+      <c r="D62" t="s">
+        <v>27</v>
+      </c>
+      <c r="E62" t="s">
+        <v>25</v>
+      </c>
+      <c r="F62" t="s">
+        <v>58</v>
+      </c>
+      <c r="G62" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C63" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" t="s">
+        <v>99</v>
+      </c>
+      <c r="E63" t="s">
+        <v>25</v>
+      </c>
+      <c r="F63" t="s">
+        <v>63</v>
+      </c>
+      <c r="G63" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" t="s">
+        <v>100</v>
+      </c>
+      <c r="E64" t="s">
+        <v>25</v>
+      </c>
+      <c r="F64" t="s">
+        <v>63</v>
+      </c>
+      <c r="G64" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" t="s">
+        <v>95</v>
+      </c>
+      <c r="E65" t="s">
+        <v>25</v>
+      </c>
+      <c r="F65" t="s">
+        <v>32</v>
+      </c>
+      <c r="G65" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" t="s">
+        <v>96</v>
+      </c>
+      <c r="E66" t="s">
+        <v>25</v>
+      </c>
+      <c r="F66" t="s">
+        <v>32</v>
+      </c>
+      <c r="G66" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" t="s">
+        <v>90</v>
+      </c>
+      <c r="E67" t="s">
+        <v>25</v>
+      </c>
+      <c r="F67" t="s">
+        <v>32</v>
+      </c>
+      <c r="G67" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C68" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68" t="s">
+        <v>91</v>
+      </c>
+      <c r="E68" t="s">
+        <v>25</v>
+      </c>
+      <c r="F68" t="s">
+        <v>32</v>
+      </c>
+      <c r="G68" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C69" t="s">
         <v>26</v>
       </c>
-      <c r="D29" t="s">
-        <v>25</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="D69" t="s">
+        <v>106</v>
+      </c>
+      <c r="E69" t="s">
+        <v>25</v>
+      </c>
+      <c r="F69" t="s">
         <v>59</v>
       </c>
-      <c r="F29" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>25</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="G69" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C70" t="s">
+        <v>33</v>
+      </c>
+      <c r="D70" t="s">
+        <v>110</v>
+      </c>
+      <c r="E70" t="s">
+        <v>25</v>
+      </c>
+      <c r="F70" t="s">
+        <v>58</v>
+      </c>
+      <c r="G70" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
+        <v>70</v>
+      </c>
+      <c r="D72" t="s">
+        <v>102</v>
+      </c>
+      <c r="E72" t="s">
+        <v>58</v>
+      </c>
+      <c r="F72" t="s">
+        <v>63</v>
+      </c>
+      <c r="G72" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C74" t="s">
+        <v>65</v>
+      </c>
+      <c r="D74" t="s">
+        <v>126</v>
+      </c>
+      <c r="E74" t="s">
+        <v>63</v>
+      </c>
+      <c r="F74" t="s">
+        <v>32</v>
+      </c>
+      <c r="G74" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C75" t="s">
+        <v>69</v>
+      </c>
+      <c r="D75" t="s">
+        <v>127</v>
+      </c>
+      <c r="E75" t="s">
+        <v>63</v>
+      </c>
+      <c r="F75" t="s">
+        <v>32</v>
+      </c>
+      <c r="G75" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C77" t="s">
+        <v>49</v>
+      </c>
+      <c r="D77" t="s">
+        <v>97</v>
+      </c>
+      <c r="E77" t="s">
+        <v>32</v>
+      </c>
+      <c r="F77" t="s">
         <v>59</v>
       </c>
-      <c r="F30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" t="s">
-        <v>25</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="G77" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C78" t="s">
+        <v>66</v>
+      </c>
+      <c r="D78" t="s">
+        <v>130</v>
+      </c>
+      <c r="E78" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C79" t="s">
+        <v>67</v>
+      </c>
+      <c r="D79" t="s">
+        <v>131</v>
+      </c>
+      <c r="E79" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C80" t="s">
+        <v>68</v>
+      </c>
+      <c r="D80" t="s">
+        <v>132</v>
+      </c>
+      <c r="E80" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C81" t="s">
+        <v>71</v>
+      </c>
+      <c r="D81" t="s">
+        <v>71</v>
+      </c>
+      <c r="E81" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
         <v>59</v>
       </c>
-      <c r="F31" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C32" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" t="s">
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C83" t="s">
+        <v>51</v>
+      </c>
+      <c r="D83" t="s">
+        <v>109</v>
+      </c>
+      <c r="E83" t="s">
         <v>59</v>
       </c>
-      <c r="F32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C33" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33" t="s">
-        <v>25</v>
-      </c>
-      <c r="E33" t="s">
-        <v>59</v>
-      </c>
-      <c r="F33" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C34" t="s">
-        <v>49</v>
-      </c>
-      <c r="D34" t="s">
-        <v>25</v>
-      </c>
-      <c r="E34" t="s">
-        <v>72</v>
-      </c>
-      <c r="F34" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C36" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" t="s">
-        <v>72</v>
-      </c>
-      <c r="E36" t="s">
-        <v>58</v>
-      </c>
-      <c r="F36" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C37" t="s">
-        <v>33</v>
-      </c>
-      <c r="D37" t="s">
-        <v>72</v>
-      </c>
-      <c r="E37" t="s">
-        <v>58</v>
-      </c>
-      <c r="F37" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C38" t="s">
-        <v>57</v>
-      </c>
-      <c r="D38" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C39" t="s">
-        <v>51</v>
-      </c>
-      <c r="D39" t="s">
-        <v>72</v>
-      </c>
-      <c r="E39" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C41" t="s">
-        <v>27</v>
-      </c>
-      <c r="D41" t="s">
-        <v>25</v>
-      </c>
-      <c r="E41" t="s">
-        <v>58</v>
-      </c>
-      <c r="F41" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C42" t="s">
-        <v>52</v>
-      </c>
-      <c r="D42" t="s">
-        <v>25</v>
-      </c>
-      <c r="E42" t="s">
-        <v>58</v>
-      </c>
-      <c r="F42" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C43" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" t="s">
-        <v>25</v>
-      </c>
-      <c r="E43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F43" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C44" t="s">
-        <v>31</v>
-      </c>
-      <c r="D44" t="s">
-        <v>25</v>
-      </c>
-      <c r="E44" t="s">
-        <v>32</v>
-      </c>
-      <c r="F44" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C46" t="s">
-        <v>34</v>
-      </c>
-      <c r="D46" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C47" t="s">
-        <v>35</v>
-      </c>
-      <c r="D47" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C48" t="s">
-        <v>36</v>
-      </c>
-      <c r="D48" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C49" t="s">
-        <v>37</v>
-      </c>
-      <c r="D49" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C50" t="s">
-        <v>38</v>
-      </c>
-      <c r="D50" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C51" t="s">
-        <v>39</v>
-      </c>
-      <c r="D51" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C52" t="s">
-        <v>41</v>
-      </c>
-      <c r="D52" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C53" t="s">
-        <v>42</v>
-      </c>
-      <c r="D53" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C54" t="s">
-        <v>43</v>
-      </c>
-      <c r="D54" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C55" t="s">
-        <v>44</v>
-      </c>
-      <c r="D55" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C56" t="s">
-        <v>45</v>
-      </c>
-      <c r="D56" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C57" t="s">
-        <v>46</v>
-      </c>
-      <c r="D57" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C58" t="s">
-        <v>47</v>
-      </c>
-      <c r="D58" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C59" t="s">
-        <v>48</v>
-      </c>
-      <c r="D59" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C60" t="s">
-        <v>50</v>
-      </c>
-      <c r="D60" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B62" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C63" t="s">
-        <v>27</v>
-      </c>
-      <c r="D63" t="s">
-        <v>25</v>
-      </c>
-      <c r="E63" t="s">
-        <v>58</v>
-      </c>
-      <c r="F63" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C64" t="s">
-        <v>8</v>
-      </c>
-      <c r="D64" t="s">
-        <v>25</v>
-      </c>
-      <c r="E64" t="s">
-        <v>63</v>
-      </c>
-      <c r="F64" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C65" t="s">
-        <v>18</v>
-      </c>
-      <c r="D65" t="s">
-        <v>25</v>
-      </c>
-      <c r="E65" t="s">
-        <v>63</v>
-      </c>
-      <c r="F65" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C66" t="s">
-        <v>13</v>
-      </c>
-      <c r="D66" t="s">
-        <v>25</v>
-      </c>
-      <c r="E66" t="s">
-        <v>32</v>
-      </c>
-      <c r="F66" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C67" t="s">
-        <v>14</v>
-      </c>
-      <c r="D67" t="s">
-        <v>25</v>
-      </c>
-      <c r="E67" t="s">
-        <v>32</v>
-      </c>
-      <c r="F67" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C68" t="s">
-        <v>6</v>
-      </c>
-      <c r="D68" t="s">
-        <v>25</v>
-      </c>
-      <c r="E68" t="s">
-        <v>32</v>
-      </c>
-      <c r="F68" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C69" t="s">
-        <v>10</v>
-      </c>
-      <c r="D69" t="s">
-        <v>25</v>
-      </c>
-      <c r="E69" t="s">
-        <v>32</v>
-      </c>
-      <c r="F69" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C70" t="s">
-        <v>26</v>
-      </c>
-      <c r="D70" t="s">
-        <v>25</v>
-      </c>
-      <c r="E70" t="s">
-        <v>59</v>
-      </c>
-      <c r="F70" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C71" t="s">
-        <v>33</v>
-      </c>
-      <c r="D71" t="s">
-        <v>25</v>
-      </c>
-      <c r="E71" t="s">
-        <v>58</v>
-      </c>
-      <c r="F71" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B72" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C73" t="s">
-        <v>70</v>
-      </c>
-      <c r="D73" t="s">
-        <v>58</v>
-      </c>
-      <c r="E73" t="s">
-        <v>63</v>
-      </c>
-      <c r="F73" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B74" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C75" t="s">
-        <v>65</v>
-      </c>
-      <c r="D75" t="s">
-        <v>63</v>
-      </c>
-      <c r="E75" t="s">
-        <v>32</v>
-      </c>
-      <c r="F75" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C76" t="s">
-        <v>69</v>
-      </c>
-      <c r="D76" t="s">
-        <v>63</v>
-      </c>
-      <c r="E76" t="s">
-        <v>32</v>
-      </c>
-      <c r="F76" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B77" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C78" t="s">
-        <v>49</v>
-      </c>
-      <c r="D78" t="s">
-        <v>32</v>
-      </c>
-      <c r="E78" t="s">
-        <v>59</v>
-      </c>
-      <c r="F78" t="s">
+      <c r="F83" t="s">
+        <v>58</v>
+      </c>
+      <c r="G83" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C79" t="s">
-        <v>66</v>
-      </c>
-      <c r="D79" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C80" t="s">
-        <v>67</v>
-      </c>
-      <c r="D80" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C81" t="s">
-        <v>68</v>
-      </c>
-      <c r="D81" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C82" t="s">
-        <v>71</v>
-      </c>
-      <c r="D82" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B83" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C84" t="s">
-        <v>51</v>
-      </c>
-      <c r="D84" t="s">
-        <v>59</v>
-      </c>
-      <c r="E84" t="s">
-        <v>58</v>
-      </c>
-      <c r="F84" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified source code to enable generic webmod names to facilitate pest runs on PC and Unix. Also modified names and contents of control file in andcrk_pest directory which is our test area.
git-svn-id: svn://136.177.114.72/svn_GW/webmod/trunk@9852 1feff8c3-07ed-0310-ac33-dd36852eb9cd
</commit_message>
<xml_diff>
--- a/pest/PestFiles.xlsx
+++ b/pest/PestFiles.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programs\webmod-trunk\pest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\System\Users\rmwebb\Desktop\webmod\pest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16848" windowHeight="10980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16845" windowHeight="10980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="173">
   <si>
     <t>AndChemLoads.ssf</t>
   </si>
@@ -421,6 +421,129 @@
   </si>
   <si>
     <t>webmod.hydro.obs.ssf</t>
+  </si>
+  <si>
+    <t>Ancillary files in webmod.control</t>
+  </si>
+  <si>
+    <t>control string</t>
+  </si>
+  <si>
+    <t>data_file</t>
+  </si>
+  <si>
+    <t>ani_output_file</t>
+  </si>
+  <si>
+    <t>reserved &amp; required</t>
+  </si>
+  <si>
+    <t>chem_file</t>
+  </si>
+  <si>
+    <t>model_output_file</t>
+  </si>
+  <si>
+    <t>model_chemout_file</t>
+  </si>
+  <si>
+    <t>input_dir</t>
+  </si>
+  <si>
+    <t>phreeq_lut is located here</t>
+  </si>
+  <si>
+    <t>phreeq_web_lite.dat is located here</t>
+  </si>
+  <si>
+    <t>output_dir</t>
+  </si>
+  <si>
+    <t>select_mixes</t>
+  </si>
+  <si>
+    <t>select mixes from phreeq written here</t>
+  </si>
+  <si>
+    <t>v_olume viles written here</t>
+  </si>
+  <si>
+    <t>s_olute files written here</t>
+  </si>
+  <si>
+    <t>e_ntity files written here</t>
+  </si>
+  <si>
+    <t>v_*</t>
+  </si>
+  <si>
+    <t>s_*</t>
+  </si>
+  <si>
+    <t>e_*</t>
+  </si>
+  <si>
+    <t>model_topout_file</t>
+  </si>
+  <si>
+    <t>param_file</t>
+  </si>
+  <si>
+    <t>phreeq_file</t>
+  </si>
+  <si>
+    <t>stat_var_file</t>
+  </si>
+  <si>
+    <t>var_init_file</t>
+  </si>
+  <si>
+    <t>webmod.var_in</t>
+  </si>
+  <si>
+    <t>webmod.aniout</t>
+  </si>
+  <si>
+    <t>var_save_file</t>
+  </si>
+  <si>
+    <t>opt_output_file</t>
+  </si>
+  <si>
+    <t>webmod.var_save</t>
+  </si>
+  <si>
+    <t>webmod.optim</t>
+  </si>
+  <si>
+    <t>param_print_file</t>
+  </si>
+  <si>
+    <t>webmod.paramprint</t>
+  </si>
+  <si>
+    <t>sens_output_file</t>
+  </si>
+  <si>
+    <t>webmod.sensout</t>
+  </si>
+  <si>
+    <t>var_print_file</t>
+  </si>
+  <si>
+    <t>webmod.varprint</t>
+  </si>
+  <si>
+    <t>gis_output_file</t>
+  </si>
+  <si>
+    <t>webmod.gisout</t>
+  </si>
+  <si>
+    <t>stats_output_file</t>
+  </si>
+  <si>
+    <t>webmod.statistics</t>
   </si>
 </sst>
 </file>
@@ -436,12 +559,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -456,8 +585,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,175 +869,181 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:H99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D61" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="F68" sqref="F67:F68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="4" width="31.21875" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" customWidth="1"/>
-    <col min="7" max="7" width="36.88671875" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" customWidth="1"/>
+    <col min="3" max="4" width="31.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="8" max="8" width="36.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>80</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>81</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>85</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>89</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C2" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>98</v>
       </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>130</v>
       </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>90</v>
       </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>111</v>
       </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>112</v>
       </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>91</v>
       </c>
-      <c r="E9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>131</v>
       </c>
-      <c r="E10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
         <v>4</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>101</v>
       </c>
-      <c r="E11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C12" t="s">
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>104</v>
       </c>
-      <c r="E12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>98</v>
-      </c>
-      <c r="E13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
-        <v>16</v>
       </c>
       <c r="D14" t="s">
         <v>98</v>
@@ -916,132 +1052,138 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
         <v>17</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>93</v>
       </c>
-      <c r="E15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
         <v>3</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>94</v>
       </c>
-      <c r="E16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
         <v>6</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>95</v>
       </c>
-      <c r="E17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" t="s">
+        <v>140</v>
+      </c>
+      <c r="H18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
         <v>10</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>96</v>
       </c>
-      <c r="E18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" t="s">
+        <v>140</v>
+      </c>
+      <c r="H19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
         <v>18</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>105</v>
       </c>
-      <c r="E19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>19</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>19</v>
       </c>
-      <c r="E20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
         <v>21</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>102</v>
       </c>
-      <c r="E22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
+      <c r="E23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
         <v>22</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>22</v>
       </c>
-      <c r="E23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="E24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>26</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>103</v>
-      </c>
-      <c r="E26" t="s">
-        <v>25</v>
-      </c>
-      <c r="F26" t="s">
-        <v>59</v>
-      </c>
-      <c r="G26" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D27" t="s">
-        <v>98</v>
       </c>
       <c r="E27" t="s">
         <v>25</v>
@@ -1049,16 +1191,16 @@
       <c r="F27" t="s">
         <v>59</v>
       </c>
-      <c r="G27" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>131</v>
+        <v>98</v>
       </c>
       <c r="E28" t="s">
         <v>25</v>
@@ -1066,16 +1208,16 @@
       <c r="F28" t="s">
         <v>59</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E29" t="s">
         <v>25</v>
@@ -1083,16 +1225,16 @@
       <c r="F29" t="s">
         <v>59</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>101</v>
+        <v>130</v>
       </c>
       <c r="E30" t="s">
         <v>25</v>
@@ -1100,16 +1242,16 @@
       <c r="F30" t="s">
         <v>59</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="E31" t="s">
         <v>25</v>
@@ -1117,16 +1259,16 @@
       <c r="F31" t="s">
         <v>59</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E32" t="s">
         <v>25</v>
@@ -1134,55 +1276,55 @@
       <c r="F32" t="s">
         <v>59</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" t="s">
+        <v>59</v>
+      </c>
+      <c r="H33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>49</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>91</v>
       </c>
-      <c r="E33" t="s">
-        <v>25</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" t="s">
         <v>72</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H34" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C35" t="s">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
         <v>40</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>92</v>
-      </c>
-      <c r="E35" t="s">
-        <v>72</v>
-      </c>
-      <c r="F35" t="s">
-        <v>58</v>
-      </c>
-      <c r="G35" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C36" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" t="s">
-        <v>114</v>
       </c>
       <c r="E36" t="s">
         <v>72</v>
@@ -1190,97 +1332,97 @@
       <c r="F36" t="s">
         <v>58</v>
       </c>
-      <c r="G36" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
       <c r="E37" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F37" t="s">
+        <v>58</v>
+      </c>
+      <c r="H37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D38" t="s">
-        <v>113</v>
+        <v>57</v>
       </c>
       <c r="E38" t="s">
         <v>72</v>
       </c>
-      <c r="F38" t="s">
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" t="s">
+        <v>113</v>
+      </c>
+      <c r="E39" t="s">
+        <v>72</v>
+      </c>
+      <c r="F39" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C40" t="s">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
         <v>27</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>27</v>
       </c>
-      <c r="E40" t="s">
-        <v>25</v>
-      </c>
-      <c r="F40" t="s">
-        <v>58</v>
-      </c>
-      <c r="G40" t="s">
+      <c r="E41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" t="s">
+        <v>58</v>
+      </c>
+      <c r="H41" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C41" t="s">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
         <v>52</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>52</v>
       </c>
-      <c r="E41" t="s">
-        <v>25</v>
-      </c>
-      <c r="F41" t="s">
-        <v>58</v>
-      </c>
-      <c r="G41" t="s">
+      <c r="E42" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" t="s">
+        <v>58</v>
+      </c>
+      <c r="H42" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C42" t="s">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
         <v>7</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>90</v>
-      </c>
-      <c r="E42" t="s">
-        <v>25</v>
-      </c>
-      <c r="F42" t="s">
-        <v>32</v>
-      </c>
-      <c r="G42" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C43" t="s">
-        <v>31</v>
-      </c>
-      <c r="D43" t="s">
-        <v>31</v>
       </c>
       <c r="E43" t="s">
         <v>25</v>
@@ -1288,230 +1430,230 @@
       <c r="F43" t="s">
         <v>32</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" t="s">
+        <v>31</v>
+      </c>
+      <c r="E44" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H44" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C45" t="s">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
         <v>34</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>115</v>
       </c>
-      <c r="E45" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C46" t="s">
+      <c r="E46" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
         <v>35</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>116</v>
       </c>
-      <c r="E46" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C47" t="s">
+      <c r="E47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
         <v>36</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>117</v>
       </c>
-      <c r="E47" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C48" t="s">
+      <c r="E48" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
         <v>37</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>118</v>
       </c>
-      <c r="E48" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C49" t="s">
+      <c r="E49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
         <v>38</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>119</v>
       </c>
-      <c r="E49" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C50" t="s">
+      <c r="E50" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
         <v>39</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>120</v>
       </c>
-      <c r="E50" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C51" t="s">
+      <c r="E51" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
         <v>41</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D52" t="s">
         <v>121</v>
       </c>
-      <c r="E51" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C52" t="s">
+      <c r="E52" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
         <v>42</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D53" t="s">
         <v>122</v>
       </c>
-      <c r="E52" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C53" t="s">
+      <c r="E53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
         <v>43</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>123</v>
       </c>
-      <c r="E53" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C54" t="s">
+      <c r="E54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
         <v>44</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>124</v>
       </c>
-      <c r="E54" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C55" t="s">
+      <c r="E55" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
         <v>45</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D56" t="s">
         <v>125</v>
       </c>
-      <c r="E55" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C56" t="s">
+      <c r="E56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
         <v>46</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>126</v>
       </c>
-      <c r="E56" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C57" t="s">
+      <c r="E57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
         <v>47</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D58" t="s">
         <v>127</v>
       </c>
-      <c r="E57" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C58" t="s">
+      <c r="E58" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
         <v>48</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>128</v>
       </c>
-      <c r="E58" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C59" t="s">
+      <c r="E59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
         <v>50</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D60" t="s">
         <v>129</v>
       </c>
-      <c r="E59" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+      <c r="E60" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B61" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C62" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
         <v>27</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D63" t="s">
         <v>27</v>
       </c>
-      <c r="E62" t="s">
-        <v>25</v>
-      </c>
-      <c r="F62" t="s">
-        <v>58</v>
-      </c>
-      <c r="G62" t="s">
+      <c r="E63" t="s">
+        <v>25</v>
+      </c>
+      <c r="F63" t="s">
+        <v>58</v>
+      </c>
+      <c r="H63" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C63" t="s">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
         <v>8</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D64" t="s">
         <v>104</v>
-      </c>
-      <c r="E63" t="s">
-        <v>25</v>
-      </c>
-      <c r="F63" t="s">
-        <v>63</v>
-      </c>
-      <c r="G63" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C64" t="s">
-        <v>18</v>
-      </c>
-      <c r="D64" t="s">
-        <v>105</v>
       </c>
       <c r="E64" t="s">
         <v>25</v>
@@ -1519,33 +1661,33 @@
       <c r="F64" t="s">
         <v>63</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65" t="s">
+        <v>105</v>
+      </c>
+      <c r="E65" t="s">
+        <v>25</v>
+      </c>
+      <c r="F65" t="s">
+        <v>63</v>
+      </c>
+      <c r="H65" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
         <v>13</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D66" t="s">
         <v>111</v>
-      </c>
-      <c r="E65" t="s">
-        <v>25</v>
-      </c>
-      <c r="F65" t="s">
-        <v>32</v>
-      </c>
-      <c r="G65" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C66" t="s">
-        <v>14</v>
-      </c>
-      <c r="D66" t="s">
-        <v>112</v>
       </c>
       <c r="E66" t="s">
         <v>25</v>
@@ -1553,16 +1695,19 @@
       <c r="F66" t="s">
         <v>32</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G66" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H66" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D67" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="E67" t="s">
         <v>25</v>
@@ -1571,15 +1716,18 @@
         <v>32</v>
       </c>
       <c r="G67" t="s">
+        <v>137</v>
+      </c>
+      <c r="H67" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D68" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E68" t="s">
         <v>25</v>
@@ -1588,93 +1736,99 @@
         <v>32</v>
       </c>
       <c r="G68" t="s">
+        <v>140</v>
+      </c>
+      <c r="H68" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69" t="s">
+        <v>96</v>
+      </c>
+      <c r="E69" t="s">
+        <v>25</v>
+      </c>
+      <c r="F69" t="s">
+        <v>32</v>
+      </c>
+      <c r="G69" t="s">
+        <v>140</v>
+      </c>
+      <c r="H69" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
         <v>26</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D70" t="s">
         <v>103</v>
       </c>
-      <c r="E69" t="s">
-        <v>25</v>
-      </c>
-      <c r="F69" t="s">
+      <c r="E70" t="s">
+        <v>25</v>
+      </c>
+      <c r="F70" t="s">
         <v>59</v>
       </c>
-      <c r="G69" t="s">
+      <c r="H70" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C70" t="s">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
         <v>33</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D71" t="s">
         <v>114</v>
       </c>
-      <c r="E70" t="s">
-        <v>25</v>
-      </c>
-      <c r="F70" t="s">
-        <v>58</v>
-      </c>
-      <c r="G70" t="s">
+      <c r="E71" t="s">
+        <v>25</v>
+      </c>
+      <c r="F71" t="s">
+        <v>58</v>
+      </c>
+      <c r="H71" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B71" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C72" t="s">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
         <v>70</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D73" t="s">
         <v>97</v>
       </c>
-      <c r="E72" t="s">
-        <v>58</v>
-      </c>
-      <c r="F72" t="s">
+      <c r="E73" t="s">
+        <v>58</v>
+      </c>
+      <c r="F73" t="s">
         <v>63</v>
       </c>
-      <c r="G72" t="s">
+      <c r="H73" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B73" t="s">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C74" t="s">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
         <v>65</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D75" t="s">
         <v>106</v>
-      </c>
-      <c r="E74" t="s">
-        <v>63</v>
-      </c>
-      <c r="F74" t="s">
-        <v>32</v>
-      </c>
-      <c r="G74" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C75" t="s">
-        <v>69</v>
-      </c>
-      <c r="D75" t="s">
-        <v>107</v>
       </c>
       <c r="E75" t="s">
         <v>63</v>
@@ -1683,99 +1837,256 @@
         <v>32</v>
       </c>
       <c r="G75" t="s">
+        <v>154</v>
+      </c>
+      <c r="H75" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>69</v>
+      </c>
+      <c r="D76" t="s">
+        <v>107</v>
+      </c>
+      <c r="E76" t="s">
+        <v>63</v>
+      </c>
+      <c r="F76" t="s">
+        <v>32</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H76" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B76" t="s">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C77" t="s">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
         <v>49</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D78" t="s">
         <v>91</v>
-      </c>
-      <c r="E77" t="s">
-        <v>32</v>
-      </c>
-      <c r="F77" t="s">
-        <v>59</v>
-      </c>
-      <c r="G77" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C78" t="s">
-        <v>66</v>
-      </c>
-      <c r="D78" t="s">
-        <v>109</v>
       </c>
       <c r="E78" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F78" t="s">
+        <v>59</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H78" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D79" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E79" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G79" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D80" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E80" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G80" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D81" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="E81" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B82" t="s">
+      <c r="G81" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>71</v>
+      </c>
+      <c r="D82" t="s">
+        <v>71</v>
+      </c>
+      <c r="E82" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C83" t="s">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
         <v>51</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D84" t="s">
         <v>113</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E84" t="s">
         <v>59</v>
       </c>
-      <c r="F83" t="s">
-        <v>58</v>
-      </c>
-      <c r="G83" t="s">
+      <c r="F84" t="s">
+        <v>58</v>
+      </c>
+      <c r="H84" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>144</v>
+      </c>
+      <c r="G87" t="s">
+        <v>143</v>
+      </c>
+      <c r="H87" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
+        <v>149</v>
+      </c>
+      <c r="G88" t="s">
+        <v>143</v>
+      </c>
+      <c r="H88" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
+        <v>150</v>
+      </c>
+      <c r="G89" t="s">
+        <v>143</v>
+      </c>
+      <c r="H89" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>151</v>
+      </c>
+      <c r="G90" t="s">
+        <v>143</v>
+      </c>
+      <c r="H90" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>158</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
+        <v>157</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>161</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>162</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
+        <v>164</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>166</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="97" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>168</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="98" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
+        <v>170</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="99" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>172</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1787,16 +2098,16 @@
       <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.21875" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="35.6640625" customWidth="1"/>
-    <col min="6" max="6" width="32.5546875" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -1807,12 +2118,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1820,7 +2131,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -1828,7 +2139,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -1836,7 +2147,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -1844,7 +2155,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>13</v>
       </c>
@@ -1852,7 +2163,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -1860,7 +2171,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -1868,7 +2179,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -1876,7 +2187,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -1884,7 +2195,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -1892,7 +2203,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -1900,7 +2211,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -1908,7 +2219,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>17</v>
       </c>
@@ -1916,7 +2227,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -1924,7 +2235,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>6</v>
       </c>
@@ -1932,7 +2243,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>10</v>
       </c>
@@ -1940,7 +2251,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>18</v>
       </c>
@@ -1948,7 +2259,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>19</v>
       </c>
@@ -1956,12 +2267,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>21</v>
       </c>
@@ -1969,7 +2280,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>22</v>
       </c>
@@ -1977,12 +2288,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>0</v>
       </c>
@@ -1993,7 +2304,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>12</v>
       </c>
@@ -2004,7 +2315,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>7</v>
       </c>
@@ -2015,7 +2326,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>13</v>
       </c>
@@ -2026,7 +2337,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>14</v>
       </c>
@@ -2037,7 +2348,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>15</v>
       </c>
@@ -2048,7 +2359,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>26</v>
       </c>
@@ -2059,7 +2370,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>1</v>
       </c>
@@ -2070,7 +2381,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>4</v>
       </c>
@@ -2081,7 +2392,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>8</v>
       </c>
@@ -2092,7 +2403,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>11</v>
       </c>
@@ -2103,7 +2414,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>16</v>
       </c>
@@ -2114,7 +2425,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>17</v>
       </c>
@@ -2125,7 +2436,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>3</v>
       </c>
@@ -2136,7 +2447,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>27</v>
       </c>
@@ -2147,7 +2458,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>6</v>
       </c>
@@ -2158,7 +2469,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>10</v>
       </c>
@@ -2169,7 +2480,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>18</v>
       </c>
@@ -2180,7 +2491,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>19</v>
       </c>
@@ -2191,7 +2502,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>31</v>
       </c>
@@ -2202,12 +2513,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>0</v>
       </c>
@@ -2218,7 +2529,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>12</v>
       </c>
@@ -2229,7 +2540,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>7</v>
       </c>
@@ -2240,7 +2551,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>13</v>
       </c>
@@ -2251,7 +2562,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>14</v>
       </c>
@@ -2262,7 +2573,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>33</v>
       </c>
@@ -2276,7 +2587,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>34</v>
       </c>
@@ -2284,7 +2595,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>35</v>
       </c>
@@ -2292,7 +2603,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>36</v>
       </c>
@@ -2300,7 +2611,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>37</v>
       </c>
@@ -2308,7 +2619,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>38</v>
       </c>
@@ -2316,7 +2627,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>39</v>
       </c>
@@ -2324,7 +2635,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>40</v>
       </c>
@@ -2335,7 +2646,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>41</v>
       </c>
@@ -2343,7 +2654,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>42</v>
       </c>
@@ -2351,7 +2662,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>43</v>
       </c>
@@ -2359,7 +2670,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>44</v>
       </c>
@@ -2367,7 +2678,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>45</v>
       </c>
@@ -2375,7 +2686,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>46</v>
       </c>
@@ -2383,7 +2694,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>47</v>
       </c>
@@ -2391,7 +2702,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>48</v>
       </c>
@@ -2399,7 +2710,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>49</v>
       </c>
@@ -2410,7 +2721,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>15</v>
       </c>
@@ -2421,7 +2732,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>50</v>
       </c>
@@ -2429,7 +2740,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>51</v>
       </c>
@@ -2443,7 +2754,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>26</v>
       </c>
@@ -2454,7 +2765,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>1</v>
       </c>
@@ -2465,7 +2776,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>4</v>
       </c>
@@ -2476,7 +2787,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>8</v>
       </c>
@@ -2487,7 +2798,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>11</v>
       </c>
@@ -2498,7 +2809,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>16</v>
       </c>
@@ -2509,7 +2820,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>17</v>
       </c>
@@ -2520,7 +2831,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>3</v>
       </c>
@@ -2531,7 +2842,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>27</v>
       </c>
@@ -2542,7 +2853,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>6</v>
       </c>
@@ -2553,7 +2864,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>10</v>
       </c>
@@ -2564,7 +2875,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>18</v>
       </c>
@@ -2575,7 +2886,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>52</v>
       </c>
@@ -2583,7 +2894,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>53</v>
       </c>
@@ -2591,7 +2902,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>54</v>
       </c>
@@ -2599,7 +2910,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>55</v>
       </c>
@@ -2607,7 +2918,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>56</v>
       </c>
@@ -2615,7 +2926,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>19</v>
       </c>
@@ -2626,7 +2937,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>57</v>
       </c>
@@ -2634,7 +2945,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>31</v>
       </c>
@@ -2642,12 +2953,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>13</v>
       </c>
@@ -2655,7 +2966,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>14</v>
       </c>
@@ -2663,7 +2974,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>26</v>
       </c>
@@ -2671,7 +2982,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>8</v>
       </c>
@@ -2679,7 +2990,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>27</v>
       </c>
@@ -2687,7 +2998,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>6</v>
       </c>
@@ -2695,7 +3006,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>10</v>
       </c>
@@ -2703,7 +3014,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>18</v>
       </c>

</xml_diff>